<commit_message>
refactoring, modify result  and readme
</commit_message>
<xml_diff>
--- a/result/WHERE_result_10fold.xlsx
+++ b/result/WHERE_result_10fold.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Repository\ta-newsX\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ACC383-C439-4D48-8591-43DF3144D57E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654517E3-8083-4554-B99F-908638AC9A8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="4090" windowHeight="6290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -138,21 +139,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -166,6 +154,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,14 +210,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2014,7 +2028,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H6"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2023,19 +2037,19 @@
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
@@ -2049,25 +2063,25 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>0.97250000000000003</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>0.93830000000000002</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>0.1111</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>0.16669999999999999</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
@@ -2078,25 +2092,25 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>0.97319999999999995</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>0.93830000000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>0.1111</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>0.16669999999999999</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="L3" t="s">
@@ -2107,42 +2121,42 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>0.9738</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>0.94440000000000002</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>0.22220000000000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>0.30769999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>0.96970000000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>0.9506</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>0.6</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>0.42859999999999998</v>
       </c>
       <c r="G5" t="s">
@@ -2163,22 +2177,22 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>0.9718</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>0.94440000000000002</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>0.5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>0.22220000000000001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>0.30769999999999997</v>
       </c>
       <c r="G6" t="s">
@@ -2199,22 +2213,22 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>0.97109999999999996</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>0.94410000000000005</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>0.125</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>0.18179999999999999</v>
       </c>
       <c r="L7" t="s">
@@ -2225,42 +2239,42 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>0.97109999999999996</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>0.93169999999999997</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>0.2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>0.125</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <v>0.15379999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>0.9718</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>0.93169999999999997</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="5">
         <v>0.2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>0.125</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="5">
         <v>0.15379999999999999</v>
       </c>
       <c r="L9" t="s">
@@ -2271,22 +2285,22 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>0.9718</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>0.94410000000000005</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>0.4</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>0.25</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="5">
         <v>0.30769999999999997</v>
       </c>
       <c r="L10" t="s">
@@ -2297,22 +2311,22 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>0.97109999999999996</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>0.94410000000000005</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <v>0.125</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="5">
         <v>0.18179999999999999</v>
       </c>
       <c r="L11" t="s">

</xml_diff>